<commit_message>
data analyses for thesis
</commit_message>
<xml_diff>
--- a/study2/order_study_data.xlsx
+++ b/study2/order_study_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trici\Documents\GitHub\thinkinghats\study2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD02754-D5D9-4221-9BBC-5F15E3D09835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7B9A5B-2F14-4C70-9110-1552C424D4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{845BFFBF-D938-DA46-B34D-49E55728430A}"/>
+    <workbookView minimized="1" xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{845BFFBF-D938-DA46-B34D-49E55728430A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$I$49</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$2:$B$5</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$C$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$C$2:$C$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$D$2:$D$5</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet2!$A$2:$B$5</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet2!$C$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet2!$C$2:$C$5</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet2!$D$2:$D$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -13690,7 +13700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C0338E-C052-8145-A484-36452DDC74C2}">
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
@@ -17811,8 +17821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A6340A-02C4-0F44-AFDE-676687A30617}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="83" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17990,7 +18000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CAEC00F-827E-9C42-8FC9-E6ECF4BF73E1}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="C42" zoomScale="75" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>

</xml_diff>